<commit_message>
Hoành thành phân tích + Usecase cấp 0
Co-Authored-By: anhtuankg1997 <anhtuankg1997@users.noreply.github.com>
Co-Authored-By: Võ Sĩ Vai <vosivai@users.noreply.github.com>
Co-Authored-By: minhtuan97 <minhtuan97@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Bao Cao/Phu Luc/Chon phuong an thiet ke.xlsx
+++ b/Bao Cao/Phu Luc/Chon phuong an thiet ke.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BF0F0559-75A1-41DD-9BD2-B79168E307C3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5D9E1418-660E-473E-8D7D-39079F3C1DA9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>Điều kiện</t>
   </si>
@@ -92,9 +92,6 @@
   </si>
   <si>
     <t>Y22</t>
-  </si>
-  <si>
-    <t>Y23</t>
   </si>
   <si>
     <t>Ràng buộc</t>
@@ -302,9 +299,6 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -321,6 +315,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -615,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,48 +624,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="8"/>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="8"/>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="7" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -685,765 +682,736 @@
       <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:8" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>20</v>
       </c>
-      <c r="C4" s="4">
-        <v>5</v>
-      </c>
-      <c r="D4" s="4">
+      <c r="C4" s="3">
+        <v>5</v>
+      </c>
+      <c r="D4" s="3">
         <f>B4*C4</f>
         <v>100</v>
       </c>
-      <c r="E4" s="4">
-        <v>5</v>
-      </c>
-      <c r="F4" s="4">
+      <c r="E4" s="3">
+        <v>5</v>
+      </c>
+      <c r="F4" s="3">
         <f>B4*E4</f>
         <v>100</v>
       </c>
-      <c r="G4" s="4">
-        <v>5</v>
-      </c>
-      <c r="H4" s="4">
+      <c r="G4" s="3">
+        <v>5</v>
+      </c>
+      <c r="H4" s="3">
         <f>B4*G4</f>
         <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>4</v>
       </c>
-      <c r="C5" s="4">
-        <v>5</v>
-      </c>
-      <c r="D5" s="4">
-        <f t="shared" ref="D5:D19" si="0">B5*C5</f>
+      <c r="C5" s="3">
+        <v>5</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" ref="D5:D18" si="0">B5*C5</f>
         <v>20</v>
       </c>
-      <c r="E5" s="4">
-        <v>5</v>
-      </c>
-      <c r="F5" s="4">
-        <f t="shared" ref="F5:F19" si="1">B5*E5</f>
+      <c r="E5" s="3">
+        <v>5</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" ref="F5:F18" si="1">B5*E5</f>
         <v>20</v>
       </c>
-      <c r="G5" s="4">
-        <v>5</v>
-      </c>
-      <c r="H5" s="4">
-        <f t="shared" ref="H5:H19" si="2">B5*G5</f>
+      <c r="G5" s="3">
+        <v>5</v>
+      </c>
+      <c r="H5" s="3">
+        <f t="shared" ref="H5:H18" si="2">B5*G5</f>
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>3</v>
       </c>
-      <c r="C6" s="4">
-        <v>5</v>
-      </c>
-      <c r="D6" s="4">
+      <c r="C6" s="3">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="E6" s="4">
-        <v>5</v>
-      </c>
-      <c r="F6" s="4">
+      <c r="E6" s="3">
+        <v>5</v>
+      </c>
+      <c r="F6" s="3">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="G6" s="4">
-        <v>5</v>
-      </c>
-      <c r="H6" s="4">
+      <c r="G6" s="3">
+        <v>5</v>
+      </c>
+      <c r="H6" s="3">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>3</v>
       </c>
-      <c r="C7" s="4">
-        <v>1</v>
-      </c>
-      <c r="D7" s="4">
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E7" s="4">
-        <v>5</v>
-      </c>
-      <c r="F7" s="4">
+      <c r="E7" s="3">
+        <v>5</v>
+      </c>
+      <c r="F7" s="3">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="G7" s="4">
-        <v>5</v>
-      </c>
-      <c r="H7" s="4">
+      <c r="G7" s="3">
+        <v>5</v>
+      </c>
+      <c r="H7" s="3">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>3</v>
       </c>
-      <c r="C8" s="4">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4">
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E8" s="4">
-        <v>5</v>
-      </c>
-      <c r="F8" s="4">
+      <c r="E8" s="3">
+        <v>5</v>
+      </c>
+      <c r="F8" s="3">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="G8" s="4">
-        <v>5</v>
-      </c>
-      <c r="H8" s="4">
+      <c r="G8" s="3">
+        <v>5</v>
+      </c>
+      <c r="H8" s="3">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>3</v>
       </c>
-      <c r="C9" s="4">
-        <v>1</v>
-      </c>
-      <c r="D9" s="4">
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E9" s="4">
-        <v>5</v>
-      </c>
-      <c r="F9" s="4">
+      <c r="E9" s="3">
+        <v>5</v>
+      </c>
+      <c r="F9" s="3">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="G9" s="4">
-        <v>5</v>
-      </c>
-      <c r="H9" s="4">
+      <c r="G9" s="3">
+        <v>5</v>
+      </c>
+      <c r="H9" s="3">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="6">
-        <v>2</v>
-      </c>
-      <c r="C10" s="4">
-        <v>1</v>
-      </c>
-      <c r="D10" s="4">
+      <c r="B10" s="5">
+        <v>2</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E10" s="4">
-        <v>1</v>
-      </c>
-      <c r="F10" s="4">
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="G10" s="4">
-        <v>5</v>
-      </c>
-      <c r="H10" s="4">
+      <c r="G10" s="3">
+        <v>5</v>
+      </c>
+      <c r="H10" s="3">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="6">
-        <v>2</v>
-      </c>
-      <c r="C11" s="4">
-        <v>1</v>
-      </c>
-      <c r="D11" s="4">
+      <c r="B11" s="5">
+        <v>2</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E11" s="4">
-        <v>1</v>
-      </c>
-      <c r="F11" s="4">
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="G11" s="4">
-        <v>5</v>
-      </c>
-      <c r="H11" s="4">
+      <c r="G11" s="3">
+        <v>5</v>
+      </c>
+      <c r="H11" s="3">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="6">
-        <v>2</v>
-      </c>
-      <c r="C12" s="4">
-        <v>1</v>
-      </c>
-      <c r="D12" s="4">
+      <c r="B12" s="5">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E12" s="4">
-        <v>1</v>
-      </c>
-      <c r="F12" s="4">
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="G12" s="4">
-        <v>5</v>
-      </c>
-      <c r="H12" s="4">
+      <c r="G12" s="3">
+        <v>5</v>
+      </c>
+      <c r="H12" s="3">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="6">
-        <v>2</v>
-      </c>
-      <c r="C13" s="4">
-        <v>1</v>
-      </c>
-      <c r="D13" s="4">
+      <c r="B13" s="5">
+        <v>2</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E13" s="4">
-        <v>1</v>
-      </c>
-      <c r="F13" s="4">
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="G13" s="4">
-        <v>5</v>
-      </c>
-      <c r="H13" s="4">
+      <c r="G13" s="3">
+        <v>5</v>
+      </c>
+      <c r="H13" s="3">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="6">
-        <v>1</v>
-      </c>
-      <c r="C14" s="4">
-        <v>1</v>
-      </c>
-      <c r="D14" s="4">
+      <c r="B14" s="5">
+        <v>2</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E14" s="4">
-        <v>1</v>
-      </c>
-      <c r="F14" s="4">
+        <v>2</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="G14" s="4">
-        <v>5</v>
-      </c>
-      <c r="H14" s="4">
+        <v>2</v>
+      </c>
+      <c r="G14" s="3">
+        <v>5</v>
+      </c>
+      <c r="H14" s="3">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="6">
-        <v>1</v>
-      </c>
-      <c r="C15" s="4">
-        <v>1</v>
-      </c>
-      <c r="D15" s="4">
+      <c r="B15" s="5">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1</v>
+      </c>
+      <c r="D15" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E15" s="4">
-        <v>1</v>
-      </c>
-      <c r="F15" s="4">
+      <c r="E15" s="3">
+        <v>5</v>
+      </c>
+      <c r="F15" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="G15" s="4">
-        <v>5</v>
-      </c>
-      <c r="H15" s="4">
+        <v>5</v>
+      </c>
+      <c r="G15" s="3">
+        <v>5</v>
+      </c>
+      <c r="H15" s="3">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="6">
-        <v>1</v>
-      </c>
-      <c r="C16" s="4">
-        <v>1</v>
-      </c>
-      <c r="D16" s="4">
+      <c r="B16" s="5">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E16" s="4">
-        <v>5</v>
-      </c>
-      <c r="F16" s="4">
+      <c r="E16" s="3">
+        <v>1</v>
+      </c>
+      <c r="F16" s="3">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="G16" s="4">
-        <v>5</v>
-      </c>
-      <c r="H16" s="4">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3">
+        <v>5</v>
+      </c>
+      <c r="H16" s="3">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="6">
-        <v>1</v>
-      </c>
-      <c r="C17" s="4">
-        <v>1</v>
-      </c>
-      <c r="D17" s="4">
+      <c r="B17" s="5">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E17" s="4">
-        <v>1</v>
-      </c>
-      <c r="F17" s="4">
+      <c r="E17" s="3">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G17" s="4">
-        <v>5</v>
-      </c>
-      <c r="H17" s="4">
+      <c r="G17" s="3">
+        <v>5</v>
+      </c>
+      <c r="H17" s="3">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="6">
-        <v>1</v>
-      </c>
-      <c r="C18" s="4">
-        <v>1</v>
-      </c>
-      <c r="D18" s="4">
+      <c r="B18" s="5">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E18" s="4">
-        <v>1</v>
-      </c>
-      <c r="F18" s="4">
+      <c r="E18" s="3">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G18" s="4">
-        <v>5</v>
-      </c>
-      <c r="H18" s="4">
+      <c r="G18" s="3">
+        <v>5</v>
+      </c>
+      <c r="H18" s="3">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="5">
+        <f>SUM(B4:B18)</f>
+        <v>50</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="3">
+        <f>SUM(D4:D18)</f>
+        <v>158</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="3">
+        <f>SUM(F4:F18)</f>
+        <v>198</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H19" s="3">
+        <f>SUM(H4:H18)</f>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="6">
-        <v>1</v>
-      </c>
-      <c r="C19" s="4">
-        <v>1</v>
-      </c>
-      <c r="D19" s="4">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E19" s="4">
-        <v>1</v>
-      </c>
-      <c r="F19" s="4">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="G19" s="4">
-        <v>5</v>
-      </c>
-      <c r="H19" s="4">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" s="6">
-        <f>SUM(B4:B19)</f>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="11"/>
+    </row>
+    <row r="21" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="2">
+        <v>10</v>
+      </c>
+      <c r="C21" s="3">
+        <v>5</v>
+      </c>
+      <c r="D21" s="3">
+        <f>B21*C21</f>
         <v>50</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="4">
-        <f>SUM(D4:D19)</f>
-        <v>158</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F20" s="4">
-        <f>SUM(F4:F19)</f>
-        <v>198</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H20" s="4">
-        <f>SUM(H4:H19)</f>
-        <v>250</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A21" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="11"/>
+      <c r="E21" s="3">
+        <v>4</v>
+      </c>
+      <c r="F21" s="3">
+        <f>B21*E21</f>
+        <v>40</v>
+      </c>
+      <c r="G21" s="3">
+        <v>2</v>
+      </c>
+      <c r="H21" s="3">
+        <f>B21*G21</f>
+        <v>20</v>
+      </c>
     </row>
     <row r="22" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="3">
-        <v>10</v>
-      </c>
-      <c r="C22" s="4">
-        <v>5</v>
-      </c>
-      <c r="D22" s="4">
-        <f>B22*C22</f>
-        <v>50</v>
-      </c>
-      <c r="E22" s="4">
+      <c r="B22" s="5">
+        <v>8</v>
+      </c>
+      <c r="C22" s="3">
+        <v>5</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" ref="D22:D27" si="3">B22*C22</f>
+        <v>40</v>
+      </c>
+      <c r="E22" s="3">
         <v>4</v>
       </c>
-      <c r="F22" s="4">
-        <f>B22*E22</f>
-        <v>40</v>
-      </c>
-      <c r="G22" s="4">
-        <v>2</v>
-      </c>
-      <c r="H22" s="4">
-        <f>B22*G22</f>
-        <v>20</v>
+      <c r="F22" s="3">
+        <f t="shared" ref="F22:F27" si="4">B22*E22</f>
+        <v>32</v>
+      </c>
+      <c r="G22" s="3">
+        <v>2</v>
+      </c>
+      <c r="H22" s="3">
+        <f t="shared" ref="H22:H27" si="5">B22*G22</f>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="5">
         <v>8</v>
       </c>
-      <c r="C23" s="4">
-        <v>5</v>
-      </c>
-      <c r="D23" s="4">
-        <f t="shared" ref="D23:D28" si="3">B23*C23</f>
-        <v>40</v>
-      </c>
-      <c r="E23" s="4">
-        <v>4</v>
-      </c>
-      <c r="F23" s="4">
-        <f t="shared" ref="F23:F28" si="4">B23*E23</f>
-        <v>32</v>
-      </c>
-      <c r="G23" s="4">
-        <v>2</v>
-      </c>
-      <c r="H23" s="4">
-        <f t="shared" ref="H23:H28" si="5">B23*G23</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="6">
-        <v>8</v>
-      </c>
-      <c r="C24" s="4">
-        <v>2</v>
-      </c>
-      <c r="D24" s="4">
+      <c r="C23" s="3">
+        <v>2</v>
+      </c>
+      <c r="D23" s="3">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E23" s="3">
         <v>4</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F23" s="3">
         <f t="shared" si="4"/>
         <v>32</v>
       </c>
-      <c r="G24" s="4">
-        <v>5</v>
-      </c>
-      <c r="H24" s="4">
+      <c r="G23" s="3">
+        <v>5</v>
+      </c>
+      <c r="H23" s="3">
         <f t="shared" si="5"/>
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="6">
+    <row r="24" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="5">
         <v>8</v>
       </c>
-      <c r="C25" s="4">
-        <v>5</v>
-      </c>
-      <c r="D25" s="4">
+      <c r="C24" s="3">
+        <v>5</v>
+      </c>
+      <c r="D24" s="3">
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="E25" s="4">
-        <v>5</v>
-      </c>
-      <c r="F25" s="4">
+      <c r="E24" s="3">
+        <v>5</v>
+      </c>
+      <c r="F24" s="3">
         <f t="shared" si="4"/>
         <v>40</v>
       </c>
-      <c r="G25" s="4">
-        <v>1</v>
-      </c>
-      <c r="H25" s="4">
+      <c r="G24" s="3">
+        <v>1</v>
+      </c>
+      <c r="H24" s="3">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="6">
+    <row r="25" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="5">
         <v>6</v>
       </c>
-      <c r="C26" s="4">
-        <v>5</v>
-      </c>
-      <c r="D26" s="4">
+      <c r="C25" s="3">
+        <v>5</v>
+      </c>
+      <c r="D25" s="3">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="E26" s="4">
-        <v>5</v>
-      </c>
-      <c r="F26" s="4">
+      <c r="E25" s="3">
+        <v>5</v>
+      </c>
+      <c r="F25" s="3">
         <f t="shared" si="4"/>
         <v>30</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G25" s="3">
         <v>3</v>
       </c>
-      <c r="H26" s="4">
+      <c r="H25" s="3">
         <f t="shared" si="5"/>
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="6">
-        <v>5</v>
-      </c>
-      <c r="C27" s="4">
-        <v>5</v>
-      </c>
-      <c r="D27" s="4">
+    <row r="26" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="5">
+        <v>5</v>
+      </c>
+      <c r="C26" s="3">
+        <v>5</v>
+      </c>
+      <c r="D26" s="3">
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="E27" s="4">
-        <v>5</v>
-      </c>
-      <c r="F27" s="4">
+      <c r="E26" s="3">
+        <v>5</v>
+      </c>
+      <c r="F26" s="3">
         <f t="shared" si="4"/>
         <v>25</v>
       </c>
-      <c r="G27" s="4">
-        <v>5</v>
-      </c>
-      <c r="H27" s="4">
+      <c r="G26" s="3">
+        <v>5</v>
+      </c>
+      <c r="H26" s="3">
         <f t="shared" si="5"/>
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" s="6">
-        <v>5</v>
-      </c>
-      <c r="C28" s="4">
-        <v>1</v>
-      </c>
-      <c r="D28" s="4">
+    <row r="27" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="5">
+        <v>5</v>
+      </c>
+      <c r="C27" s="3">
+        <v>1</v>
+      </c>
+      <c r="D27" s="3">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="E28" s="4">
+      <c r="E27" s="3">
         <v>3</v>
       </c>
-      <c r="F28" s="4">
+      <c r="F27" s="3">
         <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="G28" s="4">
-        <v>5</v>
-      </c>
-      <c r="H28" s="4">
+      <c r="G27" s="3">
+        <v>5</v>
+      </c>
+      <c r="H27" s="3">
         <f t="shared" si="5"/>
         <v>25</v>
       </c>
     </row>
+    <row r="28" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="5">
+        <f>SUM(B21:B27)</f>
+        <v>50</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="3">
+        <f>SUM(D21:D27)</f>
+        <v>206</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F28" s="3">
+        <f>SUM(F21:F27)</f>
+        <v>214</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H28" s="3">
+        <f>SUM(H21:H27)</f>
+        <v>152</v>
+      </c>
+    </row>
     <row r="29" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B29" s="6">
-        <f>SUM(B22:B28)</f>
-        <v>50</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="4">
-        <f>SUM(D22:D28)</f>
-        <v>206</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F29" s="4">
-        <f>SUM(F22:F28)</f>
-        <v>214</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H29" s="4">
-        <f>SUM(H22:H28)</f>
-        <v>152</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A30" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" s="4">
-        <f>D20+D29</f>
+      <c r="A29" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="3">
+        <f>D19+D28</f>
         <v>364</v>
       </c>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4">
-        <f t="shared" ref="E30:H30" si="6">F20+F29</f>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3">
+        <f t="shared" ref="F29:H29" si="6">F19+F28</f>
         <v>412</v>
       </c>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4">
+      <c r="G29" s="3"/>
+      <c r="H29" s="3">
         <f t="shared" si="6"/>
         <v>402</v>
       </c>
@@ -1454,7 +1422,7 @@
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A20:H20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>